<commit_message>
Created a new final quantitative excel document and included the sampling plan in it.  Edited the sampling plan by adding some titles but did not change the order.
</commit_message>
<xml_diff>
--- a/Project_Plan/Random Sampling.xlsx
+++ b/Project_Plan/Random Sampling.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21629"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21901"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Sdimo\Documents\GitHub\Sean_Acoustics\Project_Plan\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4191C6BC-624A-46E6-AFB7-6BBE35AF5CDF}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D0C3FCF5-F3F0-40A9-9976-CF9870C11828}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="20715" windowHeight="13276" activeTab="1" xr2:uid="{9C34CB48-95CF-4B00-B939-59258BE760F7}"/>
   </bookViews>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="13">
   <si>
     <t>Dates</t>
   </si>
@@ -68,13 +68,16 @@
   </si>
   <si>
     <t>20_18</t>
+  </si>
+  <si>
+    <t>Official Order</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -83,6 +86,15 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
       <u/>
       <sz val="11"/>
       <color theme="1"/>
@@ -111,10 +123,16 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="17" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -544,10 +562,13 @@
   <dimension ref="A1:E18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C9" sqref="C9"/>
+      <selection activeCell="A8" sqref="A8:A18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <cols>
+    <col min="1" max="1" width="29.796875" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A1" t="s">
@@ -624,53 +645,58 @@
         <v>0.29088045380970129</v>
       </c>
     </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A8" s="3" t="s">
+        <v>12</v>
+      </c>
+    </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="A9" t="s">
+      <c r="A9" s="4" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="A10" t="s">
+      <c r="A10" s="4" t="s">
         <v>2</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="A11" t="s">
+      <c r="A11" s="4" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="A12" t="s">
+      <c r="A12" s="4" t="s">
         <v>1</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="A13" t="s">
+      <c r="A13" s="4" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="A14" t="s">
+      <c r="A14" s="4" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="A15" t="s">
+      <c r="A15" s="4" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="A16" t="s">
+      <c r="A16" s="4" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="17" spans="1:1" x14ac:dyDescent="0.45">
-      <c r="A17" t="s">
+      <c r="A17" s="4" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="18" spans="1:1" x14ac:dyDescent="0.45">
-      <c r="A18" t="s">
+      <c r="A18" s="4" t="s">
         <v>5</v>
       </c>
     </row>
@@ -679,5 +705,6 @@
     <sortCondition descending="1" ref="B2"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>